<commit_message>
[FIX] #9, preklepy z prednasky a zle sample
</commit_message>
<xml_diff>
--- a/09-prednaska/patterns.xlsx
+++ b/09-prednaska/patterns.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16605" yWindow="9900" windowWidth="28035" windowHeight="17445" activeTab="4"/>
+    <workbookView xWindow="16605" yWindow="9900" windowWidth="28035" windowHeight="17445"/>
   </bookViews>
   <sheets>
     <sheet name="Multiple - Overview" sheetId="1" r:id="rId1"/>
@@ -1848,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3179,7 +3179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>